<commit_message>
Pobieranie pozycji od danego dostawcy z planogramu
Jako że używanie metod copy/select/paste jest silnie zależne od
widoczności obiektów, tymczasowo przełączam na metode LoadPositions
bazującą na zbieraniu porównywaniu obiektów pozycja a nie range
</commit_message>
<xml_diff>
--- a/ExcelPln2/Input/master_input.xlsx
+++ b/ExcelPln2/Input/master_input.xlsx
@@ -1054,7 +1054,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1177,6 +1177,39 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1195,35 +1228,11 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -9762,7 +9771,7 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="40" zoomScaleNormal="50" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10347,16 +10356,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="60"/>
     </row>
     <row r="3" spans="1:23" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="50">
+      <c r="C3" s="61">
         <v>1020</v>
       </c>
-      <c r="D3" s="51"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="38"/>
       <c r="N3" t="s">
         <v>164</v>
@@ -10435,27 +10444,27 @@
       <c r="A5" s="25">
         <v>1</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="55"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="54" t="s">
+      <c r="J5" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="55"/>
+      <c r="K5" s="58"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="10"/>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="60"/>
+      <c r="P5" s="52"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -10471,26 +10480,26 @@
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="54" t="s">
+      <c r="D6" s="54"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="58" t="s">
+      <c r="I6" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="55"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="58"/>
       <c r="M6" s="1" t="s">
         <v>21</v>
       </c>
@@ -10600,17 +10609,17 @@
       <c r="A8" s="31">
         <v>4</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="53"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="64"/>
       <c r="M8" s="30" t="s">
         <v>69</v>
       </c>
@@ -10872,15 +10881,14 @@
     <row r="23" ht="153" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" ht="153" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="F6:L6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="J5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="22" orientation="portrait" r:id="rId1"/>
@@ -11003,10 +11011,10 @@
     <row r="2" spans="1:29" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
+      <c r="D2" s="60"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -11036,10 +11044,10 @@
     <row r="3" spans="1:29" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="57"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -11384,10 +11392,10 @@
       <c r="T7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="U7" s="54" t="s">
+      <c r="U7" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="V7" s="55"/>
+      <c r="V7" s="58"/>
       <c r="W7" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>